<commit_message>
文字列比較用binary_less, binary_less_dic, text_less, text_less_dic を追加
</commit_message>
<xml_diff>
--- a/vh_Manual/VBAHaskell_reference.xlsx
+++ b/vh_Manual/VBAHaskell_reference.xlsx
@@ -36,6 +36,8 @@
     <definedName name="_applyFun2by2">Haskell_1_Core!$B$216</definedName>
     <definedName name="_assignVar">Haskell_2_stdFun!$B$1</definedName>
     <definedName name="_bernoulli_dist">misc_random!$B$51</definedName>
+    <definedName name="_binary_less">Haskell_5_sort!$B$235</definedName>
+    <definedName name="_binary_less_dic">Haskell_5_sort!$B$241</definedName>
     <definedName name="_bind1st">Haskell_1_Core!$B$94</definedName>
     <definedName name="_bind2nd">Haskell_1_Core!$B$102</definedName>
     <definedName name="_capacity" localSheetId="8">vh_pipe!#REF!</definedName>
@@ -173,7 +175,7 @@
     <definedName name="_mapF_imple">Haskell_0_declare!$B$22</definedName>
     <definedName name="_mapF_swap">Haskell_1_Core!$B$144</definedName>
     <definedName name="_maskVar">Haskell_2_stdFun!$B$156</definedName>
-    <definedName name="_math">Index!$A$300</definedName>
+    <definedName name="_math">Index!$A$304</definedName>
     <definedName name="_matrix_op">Index!$A$135</definedName>
     <definedName name="_max_fun">Haskell_2_stdFun!$B$222</definedName>
     <definedName name="_min_fun">Haskell_2_stdFun!$B$216</definedName>
@@ -260,7 +262,7 @@
     <definedName name="_push_n">vh_stdvec!$B$181</definedName>
     <definedName name="_random_iota">misc_random!$B$74</definedName>
     <definedName name="_random_shuffle">misc_random!$B$82</definedName>
-    <definedName name="_randoms">Index!$A$290</definedName>
+    <definedName name="_randoms">Index!$A$294</definedName>
     <definedName name="_repeat">Haskell_4_vector!$B$24</definedName>
     <definedName name="_repeat_imple">Haskell_0_declare!$B$185</definedName>
     <definedName name="_repeat_while">Haskell_1_Core!$B$261</definedName>
@@ -312,7 +314,7 @@
     <definedName name="_splitStr2Funs">misc_utility!$B$259</definedName>
     <definedName name="_stdfun">Index!$A$74</definedName>
     <definedName name="_stdsort">Haskell_0_declare!$B$159</definedName>
-    <definedName name="_stdvec">Index!$A$208</definedName>
+    <definedName name="_stdvec">Index!$A$212</definedName>
     <definedName name="_str_cat">Haskell_2_stdFun!$B$270</definedName>
     <definedName name="_str_left">Haskell_2_stdFun!$B$252</definedName>
     <definedName name="_str_len">Haskell_2_stdFun!$B$246</definedName>
@@ -332,6 +334,8 @@
     <definedName name="_swap2nd">Haskell_1_Core!$B$118</definedName>
     <definedName name="_swapVariant">Haskell_0_declare!$B$197</definedName>
     <definedName name="_tailN">Haskell_4_vector!$B$93</definedName>
+    <definedName name="_text_less">Haskell_5_sort!$B$247</definedName>
+    <definedName name="_text_less_dic">Haskell_5_sort!$B$253</definedName>
     <definedName name="_transpose">Haskell_4_vector!$B$423</definedName>
     <definedName name="_unbind_invoke">Haskell_0_declare!$B$15</definedName>
     <definedName name="_uniform_int_dist">misc_random!$B$16</definedName>
@@ -339,7 +343,7 @@
     <definedName name="_unzip">Haskell_4_vector!$B$522</definedName>
     <definedName name="_upper_bound">Haskell_5_sort!$B$115</definedName>
     <definedName name="_upper_bound_pred">Haskell_5_sort!$B$132</definedName>
-    <definedName name="_utilities">Index!$A$246</definedName>
+    <definedName name="_utilities">Index!$A$250</definedName>
     <definedName name="_val" localSheetId="8">vh_pipe!#REF!</definedName>
     <definedName name="_val">vh_stdvec!$B$150</definedName>
     <definedName name="_vba_home">Index!$A$1</definedName>
@@ -351,7 +355,7 @@
     <definedName name="_vec_printS" localSheetId="8">vh_pipe!#REF!</definedName>
     <definedName name="_vec_printS">vh_stdvec!$B$121</definedName>
     <definedName name="_vector">Haskell_4_vector!$B$104</definedName>
-    <definedName name="_vh_pipe">Index!$A$236</definedName>
+    <definedName name="_vh_pipe">Index!$A$240</definedName>
     <definedName name="_yield_0">Haskell_1_Core!$B$34</definedName>
     <definedName name="_yield_1">Haskell_1_Core!$B$41</definedName>
     <definedName name="_yield_2">Haskell_1_Core!$B$48</definedName>
@@ -366,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3063" uniqueCount="2041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3092" uniqueCount="2058">
   <si>
     <t>Dimension</t>
   </si>
@@ -25085,6 +25089,266 @@
   <si>
     <t>述語による最良値位置検索（find_best_pred関数内部で使用）</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>述語 文字列をvbBinaryCompareで比較</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p_binary_less</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>述語 辞書式binary_less</t>
+  </si>
+  <si>
+    <t>述語 辞書式binary_less</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>binary_less_dic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ByRef a As Variant, ByRef b As Variant) As Variant</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p_binary_less_dic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>述語 文字列をvbTextCompareで比較</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>text_less</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ByRef a As Variant, ByRef b As Variant) As Variant</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p_text_less</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>述語 辞書式text_less</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>text_less_dic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ByRef a As Variant, ByRef b As Variant) As Variant</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p_text_less_dic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>binary_less</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ByRef a As Variant, ByRef b As Variant) As Variant</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>binary_less</t>
+  </si>
+  <si>
+    <t>binary_less_dic</t>
+  </si>
+  <si>
+    <t>text_less</t>
+  </si>
+  <si>
+    <t>text_less_dic</t>
   </si>
 </sst>
 </file>
@@ -28002,7 +28266,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:F320"/>
+  <dimension ref="A1:F324"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -30676,199 +30940,199 @@
         <v>894</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
-      <c r="A207" s="2"/>
-      <c r="B207" s="2"/>
-      <c r="C207" s="2"/>
-      <c r="D207" s="32"/>
+    <row r="207" spans="1:4" ht="15" customHeight="1">
+      <c r="A207" s="66" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B207" s="18" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C207" s="31" t="s">
+        <v>2041</v>
+      </c>
+      <c r="D207" s="41" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="208" spans="1:4" ht="15" customHeight="1">
-      <c r="A208" s="25" t="s">
+      <c r="A208" s="66" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B208" s="18" t="s">
+        <v>2055</v>
+      </c>
+      <c r="C208" s="31" t="s">
+        <v>2043</v>
+      </c>
+      <c r="D208" s="41" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" ht="15" customHeight="1">
+      <c r="A209" s="66" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B209" s="18" t="s">
+        <v>2056</v>
+      </c>
+      <c r="C209" s="31" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D209" s="41" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="15" customHeight="1">
+      <c r="A210" s="66" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B210" s="24" t="s">
+        <v>2057</v>
+      </c>
+      <c r="C210" s="31" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D210" s="41" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="2"/>
+      <c r="B211" s="2"/>
+      <c r="C211" s="2"/>
+      <c r="D211" s="32"/>
+    </row>
+    <row r="212" spans="1:5" ht="15" customHeight="1">
+      <c r="A212" s="25" t="s">
         <v>1718</v>
       </c>
-      <c r="B208" s="26"/>
-      <c r="C208" s="42"/>
-      <c r="D208" s="43"/>
-    </row>
-    <row r="209" spans="1:5" ht="15" customHeight="1">
-      <c r="A209" s="6" t="s">
+      <c r="B212" s="26"/>
+      <c r="C212" s="42"/>
+      <c r="D212" s="43"/>
+    </row>
+    <row r="213" spans="1:5" ht="15" customHeight="1">
+      <c r="A213" s="6" t="s">
         <v>1699</v>
       </c>
-      <c r="B209" s="24" t="s">
+      <c r="B213" s="24" t="s">
         <v>1685</v>
       </c>
-      <c r="C209" s="7" t="s">
+      <c r="C213" s="7" t="s">
         <v>1686</v>
       </c>
-      <c r="D209" s="38" t="s">
+      <c r="D213" s="38" t="s">
         <v>1687</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="15" customHeight="1">
-      <c r="A210" s="8" t="s">
+    <row r="214" spans="1:5" ht="15" customHeight="1">
+      <c r="A214" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B210" s="18" t="s">
+      <c r="B214" s="18" t="s">
         <v>1722</v>
       </c>
-      <c r="C210" s="9" t="s">
+      <c r="C214" s="9" t="s">
         <v>1639</v>
       </c>
-      <c r="D210" s="38" t="s">
+      <c r="D214" s="38" t="s">
         <v>1687</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" ht="15" customHeight="1">
-      <c r="A211" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B211" s="18" t="s">
-        <v>1688</v>
-      </c>
-      <c r="C211" s="9" t="s">
-        <v>1689</v>
-      </c>
-      <c r="D211" s="38" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" ht="15" customHeight="1">
-      <c r="A212" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B212" s="18" t="s">
-        <v>1690</v>
-      </c>
-      <c r="C212" s="9" t="s">
-        <v>1640</v>
-      </c>
-      <c r="D212" s="41" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" ht="15" customHeight="1">
-      <c r="A213" s="66" t="s">
-        <v>1708</v>
-      </c>
-      <c r="B213" s="18" t="s">
-        <v>1709</v>
-      </c>
-      <c r="C213" s="9" t="s">
-        <v>1723</v>
-      </c>
-      <c r="D213" s="41" t="s">
-        <v>1687</v>
-      </c>
-      <c r="E213"/>
-    </row>
-    <row r="214" spans="1:5" ht="15" customHeight="1">
-      <c r="A214" s="66" t="s">
-        <v>1149</v>
-      </c>
-      <c r="B214" s="18" t="s">
-        <v>1735</v>
-      </c>
-      <c r="C214" s="31" t="s">
-        <v>1736</v>
-      </c>
-      <c r="D214" s="41" t="s">
-        <v>1687</v>
-      </c>
-      <c r="E214"/>
     </row>
     <row r="215" spans="1:5" ht="15" customHeight="1">
       <c r="A215" s="8" t="s">
-        <v>1700</v>
+        <v>1</v>
       </c>
       <c r="B215" s="18" t="s">
-        <v>1692</v>
+        <v>1688</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>1691</v>
-      </c>
-      <c r="D215" s="41" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D215" s="38" t="s">
         <v>1687</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="15" customHeight="1">
       <c r="A216" s="8" t="s">
-        <v>1700</v>
+        <v>1</v>
       </c>
       <c r="B216" s="18" t="s">
-        <v>1694</v>
+        <v>1690</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>1693</v>
+        <v>1640</v>
       </c>
       <c r="D216" s="41" t="s">
         <v>1687</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="15" customHeight="1">
-      <c r="A217" s="8" t="s">
-        <v>1</v>
+      <c r="A217" s="66" t="s">
+        <v>1708</v>
       </c>
       <c r="B217" s="18" t="s">
-        <v>1695</v>
-      </c>
-      <c r="C217" s="10" t="s">
-        <v>1593</v>
+        <v>1709</v>
+      </c>
+      <c r="C217" s="9" t="s">
+        <v>1723</v>
       </c>
       <c r="D217" s="41" t="s">
         <v>1687</v>
       </c>
+      <c r="E217"/>
     </row>
     <row r="218" spans="1:5" ht="15" customHeight="1">
-      <c r="A218" s="8" t="s">
-        <v>1</v>
+      <c r="A218" s="66" t="s">
+        <v>1149</v>
       </c>
       <c r="B218" s="18" t="s">
-        <v>1696</v>
+        <v>1735</v>
       </c>
       <c r="C218" s="31" t="s">
-        <v>1595</v>
+        <v>1736</v>
       </c>
       <c r="D218" s="41" t="s">
         <v>1687</v>
       </c>
+      <c r="E218"/>
     </row>
     <row r="219" spans="1:5" ht="15" customHeight="1">
-      <c r="A219" s="66" t="s">
-        <v>1698</v>
+      <c r="A219" s="8" t="s">
+        <v>1700</v>
       </c>
       <c r="B219" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C219" s="10" t="s">
-        <v>1669</v>
+        <v>1692</v>
+      </c>
+      <c r="C219" s="9" t="s">
+        <v>1691</v>
       </c>
       <c r="D219" s="41" t="s">
         <v>1687</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="15" customHeight="1">
-      <c r="A220" s="66" t="s">
-        <v>1698</v>
+      <c r="A220" s="8" t="s">
+        <v>1700</v>
       </c>
       <c r="B220" s="18" t="s">
-        <v>1697</v>
-      </c>
-      <c r="C220" s="31" t="s">
-        <v>1642</v>
+        <v>1694</v>
+      </c>
+      <c r="C220" s="9" t="s">
+        <v>1693</v>
       </c>
       <c r="D220" s="41" t="s">
         <v>1687</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="15" customHeight="1">
-      <c r="A221" s="66" t="s">
-        <v>1698</v>
+      <c r="A221" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="B221" s="18" t="s">
-        <v>1701</v>
-      </c>
-      <c r="C221" s="9" t="s">
-        <v>1577</v>
+        <v>1695</v>
+      </c>
+      <c r="C221" s="10" t="s">
+        <v>1593</v>
       </c>
       <c r="D221" s="41" t="s">
         <v>1687</v>
@@ -30876,129 +31140,125 @@
     </row>
     <row r="222" spans="1:5" ht="15" customHeight="1">
       <c r="A222" s="8" t="s">
-        <v>1700</v>
+        <v>1</v>
       </c>
       <c r="B222" s="18" t="s">
-        <v>1702</v>
+        <v>1696</v>
       </c>
       <c r="C222" s="31" t="s">
-        <v>1641</v>
+        <v>1595</v>
       </c>
       <c r="D222" s="41" t="s">
         <v>1687</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="15" customHeight="1">
-      <c r="A223" s="8" t="s">
-        <v>1700</v>
+      <c r="A223" s="66" t="s">
+        <v>1698</v>
       </c>
       <c r="B223" s="18" t="s">
-        <v>1703</v>
-      </c>
-      <c r="C223" s="9" t="s">
-        <v>1651</v>
+        <v>140</v>
+      </c>
+      <c r="C223" s="10" t="s">
+        <v>1669</v>
       </c>
       <c r="D223" s="41" t="s">
         <v>1687</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="15" customHeight="1">
-      <c r="A224" s="8" t="s">
-        <v>1</v>
+      <c r="A224" s="66" t="s">
+        <v>1698</v>
       </c>
       <c r="B224" s="18" t="s">
-        <v>1704</v>
+        <v>1697</v>
       </c>
       <c r="C224" s="31" t="s">
-        <v>1744</v>
+        <v>1642</v>
       </c>
       <c r="D224" s="41" t="s">
         <v>1687</v>
       </c>
     </row>
     <row r="225" spans="1:6" ht="15" customHeight="1">
-      <c r="A225" s="8" t="s">
+      <c r="A225" s="66" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B225" s="18" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C225" s="9" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D225" s="41" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="15" customHeight="1">
+      <c r="A226" s="8" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B226" s="18" t="s">
+        <v>1702</v>
+      </c>
+      <c r="C226" s="31" t="s">
+        <v>1641</v>
+      </c>
+      <c r="D226" s="41" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="15" customHeight="1">
+      <c r="A227" s="8" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B227" s="18" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C227" s="9" t="s">
+        <v>1651</v>
+      </c>
+      <c r="D227" s="41" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="15" customHeight="1">
+      <c r="A228" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B225" s="18" t="s">
+      <c r="B228" s="18" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C228" s="31" t="s">
+        <v>1744</v>
+      </c>
+      <c r="D228" s="41" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="15" customHeight="1">
+      <c r="A229" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B229" s="18" t="s">
         <v>1705</v>
       </c>
-      <c r="C225" s="9" t="s">
+      <c r="C229" s="9" t="s">
         <v>1581</v>
-      </c>
-      <c r="D225" s="38" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" ht="15" customHeight="1">
-      <c r="A226" s="66" t="s">
-        <v>1707</v>
-      </c>
-      <c r="B226" s="18" t="s">
-        <v>1706</v>
-      </c>
-      <c r="C226" s="9" t="s">
-        <v>1583</v>
-      </c>
-      <c r="D226" s="38" t="s">
-        <v>1687</v>
-      </c>
-      <c r="E226"/>
-    </row>
-    <row r="227" spans="1:6" ht="15" customHeight="1">
-      <c r="A227" s="66" t="s">
-        <v>1708</v>
-      </c>
-      <c r="B227" s="18" t="s">
-        <v>1710</v>
-      </c>
-      <c r="C227" s="9" t="s">
-        <v>1585</v>
-      </c>
-      <c r="D227" s="38" t="s">
-        <v>1687</v>
-      </c>
-      <c r="E227"/>
-    </row>
-    <row r="228" spans="1:6" ht="15" customHeight="1">
-      <c r="A228" s="66" t="s">
-        <v>1708</v>
-      </c>
-      <c r="B228" s="18" t="s">
-        <v>1711</v>
-      </c>
-      <c r="C228" s="9" t="s">
-        <v>1587</v>
-      </c>
-      <c r="D228" s="38" t="s">
-        <v>1687</v>
-      </c>
-      <c r="E228"/>
-    </row>
-    <row r="229" spans="1:6" ht="15" customHeight="1">
-      <c r="A229" s="66" t="s">
-        <v>1708</v>
-      </c>
-      <c r="B229" s="18" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C229" s="9" t="s">
-        <v>1589</v>
       </c>
       <c r="D229" s="38" t="s">
         <v>1687</v>
       </c>
-      <c r="E229"/>
     </row>
     <row r="230" spans="1:6" ht="15" customHeight="1">
       <c r="A230" s="66" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B230" s="18" t="s">
-        <v>1713</v>
+        <v>1706</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>1591</v>
+        <v>1583</v>
       </c>
       <c r="D230" s="38" t="s">
         <v>1687</v>
@@ -31007,162 +31267,166 @@
     </row>
     <row r="231" spans="1:6" ht="15" customHeight="1">
       <c r="A231" s="66" t="s">
-        <v>1149</v>
-      </c>
-      <c r="B231" s="24" t="s">
-        <v>2018</v>
+        <v>1708</v>
+      </c>
+      <c r="B231" s="18" t="s">
+        <v>1710</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>2019</v>
+        <v>1585</v>
       </c>
       <c r="D231" s="38" t="s">
-        <v>893</v>
+        <v>1687</v>
       </c>
       <c r="E231"/>
     </row>
-    <row r="232" spans="1:6" s="130" customFormat="1" ht="15" customHeight="1">
-      <c r="A232" s="126" t="s">
-        <v>1</v>
-      </c>
-      <c r="B232" s="131" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C232" s="127" t="s">
-        <v>1746</v>
+    <row r="232" spans="1:6" ht="15" customHeight="1">
+      <c r="A232" s="66" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B232" s="18" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C232" s="9" t="s">
+        <v>1587</v>
       </c>
       <c r="D232" s="38" t="s">
         <v>1687</v>
       </c>
-      <c r="E232" s="128"/>
-      <c r="F232" s="129"/>
-    </row>
-    <row r="233" spans="1:6" s="130" customFormat="1" ht="15" customHeight="1">
-      <c r="A233" s="126" t="s">
-        <v>1</v>
-      </c>
-      <c r="B233" s="131" t="s">
-        <v>1747</v>
-      </c>
-      <c r="C233" s="127" t="s">
-        <v>1748</v>
+      <c r="E232"/>
+    </row>
+    <row r="233" spans="1:6" ht="15" customHeight="1">
+      <c r="A233" s="66" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B233" s="18" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C233" s="9" t="s">
+        <v>1589</v>
       </c>
       <c r="D233" s="38" t="s">
         <v>1687</v>
       </c>
-      <c r="E233" s="128"/>
-      <c r="F233" s="129"/>
-    </row>
-    <row r="234" spans="1:6" s="130" customFormat="1" ht="15" customHeight="1">
-      <c r="A234" s="126" t="s">
-        <v>1</v>
-      </c>
-      <c r="B234" s="131" t="s">
-        <v>1749</v>
-      </c>
-      <c r="C234" s="127" t="s">
-        <v>1750</v>
+      <c r="E233"/>
+    </row>
+    <row r="234" spans="1:6" ht="15" customHeight="1">
+      <c r="A234" s="66" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B234" s="18" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C234" s="9" t="s">
+        <v>1591</v>
       </c>
       <c r="D234" s="38" t="s">
         <v>1687</v>
       </c>
-      <c r="E234" s="128"/>
-      <c r="F234" s="129"/>
-    </row>
-    <row r="235" spans="1:6">
-      <c r="A235" s="2"/>
-      <c r="B235" s="2"/>
-      <c r="C235" s="2"/>
-      <c r="D235" s="32"/>
-    </row>
-    <row r="236" spans="1:6" ht="15" customHeight="1">
-      <c r="A236" s="27" t="s">
-        <v>1796</v>
-      </c>
-      <c r="B236" s="26"/>
-      <c r="C236" s="42"/>
-      <c r="D236" s="43"/>
-    </row>
-    <row r="237" spans="1:6" ht="15" customHeight="1">
-      <c r="A237" s="8" t="s">
+      <c r="E234"/>
+    </row>
+    <row r="235" spans="1:6" ht="15" customHeight="1">
+      <c r="A235" s="66" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B235" s="24" t="s">
+        <v>2018</v>
+      </c>
+      <c r="C235" s="9" t="s">
+        <v>2019</v>
+      </c>
+      <c r="D235" s="38" t="s">
+        <v>893</v>
+      </c>
+      <c r="E235"/>
+    </row>
+    <row r="236" spans="1:6" s="130" customFormat="1" ht="15" customHeight="1">
+      <c r="A236" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="B237" s="18" t="s">
-        <v>1773</v>
-      </c>
-      <c r="C237" s="33" t="s">
-        <v>1797</v>
+      <c r="B236" s="131" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C236" s="127" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D236" s="38" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E236" s="128"/>
+      <c r="F236" s="129"/>
+    </row>
+    <row r="237" spans="1:6" s="130" customFormat="1" ht="15" customHeight="1">
+      <c r="A237" s="126" t="s">
+        <v>1</v>
+      </c>
+      <c r="B237" s="131" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C237" s="127" t="s">
+        <v>1748</v>
       </c>
       <c r="D237" s="38" t="s">
         <v>1687</v>
       </c>
-    </row>
-    <row r="238" spans="1:6" ht="15" customHeight="1">
-      <c r="A238" s="8" t="s">
+      <c r="E237" s="128"/>
+      <c r="F237" s="129"/>
+    </row>
+    <row r="238" spans="1:6" s="130" customFormat="1" ht="15" customHeight="1">
+      <c r="A238" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="B238" s="18" t="s">
-        <v>1775</v>
-      </c>
-      <c r="C238" s="9" t="s">
-        <v>1776</v>
+      <c r="B238" s="131" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C238" s="127" t="s">
+        <v>1750</v>
       </c>
       <c r="D238" s="38" t="s">
         <v>1687</v>
       </c>
-    </row>
-    <row r="239" spans="1:6" ht="15" customHeight="1">
-      <c r="A239" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B239" s="18" t="s">
-        <v>1798</v>
-      </c>
-      <c r="C239" s="9" t="s">
-        <v>1808</v>
-      </c>
-      <c r="D239" s="38" t="s">
-        <v>1687</v>
-      </c>
+      <c r="E238" s="128"/>
+      <c r="F238" s="129"/>
+    </row>
+    <row r="239" spans="1:6">
+      <c r="A239" s="2"/>
+      <c r="B239" s="2"/>
+      <c r="C239" s="2"/>
+      <c r="D239" s="32"/>
     </row>
     <row r="240" spans="1:6" ht="15" customHeight="1">
-      <c r="A240" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B240" s="18" t="s">
-        <v>1799</v>
-      </c>
-      <c r="C240" s="9" t="s">
-        <v>1808</v>
-      </c>
-      <c r="D240" s="41" t="s">
-        <v>1687</v>
-      </c>
+      <c r="A240" s="27" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B240" s="26"/>
+      <c r="C240" s="42"/>
+      <c r="D240" s="43"/>
     </row>
     <row r="241" spans="1:4" ht="15" customHeight="1">
       <c r="A241" s="8" t="s">
-        <v>1700</v>
+        <v>1</v>
       </c>
       <c r="B241" s="18" t="s">
-        <v>1800</v>
-      </c>
-      <c r="C241" s="9" t="s">
-        <v>1806</v>
-      </c>
-      <c r="D241" s="41" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C241" s="33" t="s">
+        <v>1797</v>
+      </c>
+      <c r="D241" s="38" t="s">
         <v>1687</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="15" customHeight="1">
       <c r="A242" s="8" t="s">
-        <v>1700</v>
+        <v>1</v>
       </c>
       <c r="B242" s="18" t="s">
-        <v>1801</v>
+        <v>1775</v>
       </c>
       <c r="C242" s="9" t="s">
-        <v>1807</v>
-      </c>
-      <c r="D242" s="41" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D242" s="38" t="s">
         <v>1687</v>
       </c>
     </row>
@@ -31171,12 +31435,12 @@
         <v>1</v>
       </c>
       <c r="B243" s="18" t="s">
-        <v>1802</v>
+        <v>1798</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>1804</v>
-      </c>
-      <c r="D243" s="41" t="s">
+        <v>1808</v>
+      </c>
+      <c r="D243" s="38" t="s">
         <v>1687</v>
       </c>
     </row>
@@ -31185,98 +31449,98 @@
         <v>1</v>
       </c>
       <c r="B244" s="18" t="s">
-        <v>1803</v>
+        <v>1799</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>1805</v>
+        <v>1808</v>
       </c>
       <c r="D244" s="41" t="s">
         <v>1687</v>
       </c>
     </row>
-    <row r="245" spans="1:4">
-      <c r="A245" s="2"/>
-      <c r="B245" s="2"/>
-      <c r="C245" s="2"/>
-      <c r="D245" s="32"/>
+    <row r="245" spans="1:4" ht="15" customHeight="1">
+      <c r="A245" s="8" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B245" s="18" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C245" s="9" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D245" s="41" t="s">
+        <v>1687</v>
+      </c>
     </row>
     <row r="246" spans="1:4" ht="15" customHeight="1">
-      <c r="A246" s="25" t="s">
-        <v>852</v>
-      </c>
-      <c r="B246" s="26"/>
-      <c r="C246" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="D246" s="32"/>
+      <c r="A246" s="8" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B246" s="18" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C246" s="9" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D246" s="41" t="s">
+        <v>1687</v>
+      </c>
     </row>
     <row r="247" spans="1:4" ht="15" customHeight="1">
-      <c r="A247" s="6" t="s">
+      <c r="A247" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B247" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="C247" s="33" t="s">
-        <v>876</v>
-      </c>
-      <c r="D247" s="69" t="s">
-        <v>893</v>
+      <c r="B247" s="18" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C247" s="9" t="s">
+        <v>1804</v>
+      </c>
+      <c r="D247" s="41" t="s">
+        <v>1687</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="15" customHeight="1">
       <c r="A248" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B248" s="65" t="s">
-        <v>862</v>
-      </c>
-      <c r="C248" s="31" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D248" s="69" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" ht="15" customHeight="1">
-      <c r="A249" s="8" t="s">
+      <c r="B248" s="18" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C248" s="9" t="s">
+        <v>1805</v>
+      </c>
+      <c r="D248" s="41" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
+      <c r="A249" s="2"/>
+      <c r="B249" s="2"/>
+      <c r="C249" s="2"/>
+      <c r="D249" s="32"/>
+    </row>
+    <row r="250" spans="1:4" ht="15" customHeight="1">
+      <c r="A250" s="25" t="s">
+        <v>852</v>
+      </c>
+      <c r="B250" s="26"/>
+      <c r="C250" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D250" s="32"/>
+    </row>
+    <row r="251" spans="1:4" ht="15" customHeight="1">
+      <c r="A251" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B249" s="65" t="s">
-        <v>1132</v>
-      </c>
-      <c r="C249" s="31" t="s">
-        <v>1130</v>
-      </c>
-      <c r="D249" s="69" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" ht="15" customHeight="1">
-      <c r="A250" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B250" s="18" t="s">
-        <v>1505</v>
-      </c>
-      <c r="C250" s="31" t="s">
-        <v>1506</v>
-      </c>
-      <c r="D250" s="69" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" ht="15" customHeight="1">
-      <c r="A251" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B251" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C251" s="31" t="s">
-        <v>877</v>
-      </c>
-      <c r="D251" s="38" t="s">
+      <c r="B251" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="C251" s="33" t="s">
+        <v>876</v>
+      </c>
+      <c r="D251" s="69" t="s">
         <v>893</v>
       </c>
     </row>
@@ -31284,13 +31548,13 @@
       <c r="A252" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B252" s="18" t="s">
-        <v>1539</v>
+      <c r="B252" s="65" t="s">
+        <v>862</v>
       </c>
       <c r="C252" s="31" t="s">
-        <v>1540</v>
-      </c>
-      <c r="D252" s="38" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D252" s="69" t="s">
         <v>893</v>
       </c>
     </row>
@@ -31298,13 +31562,13 @@
       <c r="A253" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B253" s="18" t="s">
-        <v>286</v>
+      <c r="B253" s="65" t="s">
+        <v>1132</v>
       </c>
       <c r="C253" s="31" t="s">
-        <v>878</v>
-      </c>
-      <c r="D253" s="38" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D253" s="69" t="s">
         <v>893</v>
       </c>
     </row>
@@ -31313,12 +31577,12 @@
         <v>1</v>
       </c>
       <c r="B254" s="18" t="s">
-        <v>287</v>
+        <v>1505</v>
       </c>
       <c r="C254" s="31" t="s">
-        <v>879</v>
-      </c>
-      <c r="D254" s="38" t="s">
+        <v>1506</v>
+      </c>
+      <c r="D254" s="69" t="s">
         <v>893</v>
       </c>
     </row>
@@ -31327,10 +31591,10 @@
         <v>1</v>
       </c>
       <c r="B255" s="18" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C255" s="31" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="D255" s="38" t="s">
         <v>893</v>
@@ -31340,11 +31604,11 @@
       <c r="A256" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B256" s="24" t="s">
-        <v>1907</v>
+      <c r="B256" s="18" t="s">
+        <v>1539</v>
       </c>
       <c r="C256" s="31" t="s">
-        <v>1908</v>
+        <v>1540</v>
       </c>
       <c r="D256" s="38" t="s">
         <v>893</v>
@@ -31355,10 +31619,10 @@
         <v>1</v>
       </c>
       <c r="B257" s="18" t="s">
-        <v>1537</v>
+        <v>286</v>
       </c>
       <c r="C257" s="31" t="s">
-        <v>1538</v>
+        <v>878</v>
       </c>
       <c r="D257" s="38" t="s">
         <v>893</v>
@@ -31369,10 +31633,10 @@
         <v>1</v>
       </c>
       <c r="B258" s="18" t="s">
-        <v>1837</v>
+        <v>287</v>
       </c>
       <c r="C258" s="31" t="s">
-        <v>1838</v>
+        <v>879</v>
       </c>
       <c r="D258" s="38" t="s">
         <v>893</v>
@@ -31383,27 +31647,27 @@
         <v>1</v>
       </c>
       <c r="B259" s="18" t="s">
-        <v>790</v>
-      </c>
-      <c r="C259" s="9" t="s">
-        <v>789</v>
+        <v>288</v>
+      </c>
+      <c r="C259" s="31" t="s">
+        <v>880</v>
       </c>
       <c r="D259" s="38" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="15" customHeight="1">
       <c r="A260" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B260" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="C260" s="10" t="s">
-        <v>385</v>
+      <c r="B260" s="24" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C260" s="31" t="s">
+        <v>1908</v>
       </c>
       <c r="D260" s="38" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="15" customHeight="1">
@@ -31411,13 +31675,13 @@
         <v>1</v>
       </c>
       <c r="B261" s="18" t="s">
-        <v>294</v>
+        <v>1537</v>
       </c>
       <c r="C261" s="31" t="s">
-        <v>1972</v>
+        <v>1538</v>
       </c>
       <c r="D261" s="38" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="15" customHeight="1">
@@ -31425,13 +31689,13 @@
         <v>1</v>
       </c>
       <c r="B262" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="C262" s="10" t="s">
-        <v>386</v>
+        <v>1837</v>
+      </c>
+      <c r="C262" s="31" t="s">
+        <v>1838</v>
       </c>
       <c r="D262" s="38" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="15" customHeight="1">
@@ -31439,10 +31703,10 @@
         <v>1</v>
       </c>
       <c r="B263" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="C263" s="31" t="s">
-        <v>1972</v>
+        <v>790</v>
+      </c>
+      <c r="C263" s="9" t="s">
+        <v>789</v>
       </c>
       <c r="D263" s="38" t="s">
         <v>894</v>
@@ -31453,10 +31717,10 @@
         <v>1</v>
       </c>
       <c r="B264" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="C264" s="31" t="s">
-        <v>1973</v>
+        <v>293</v>
+      </c>
+      <c r="C264" s="10" t="s">
+        <v>385</v>
       </c>
       <c r="D264" s="38" t="s">
         <v>894</v>
@@ -31467,100 +31731,104 @@
         <v>1</v>
       </c>
       <c r="B265" s="18" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C265" s="31" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="D265" s="38" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15" customHeight="1">
-      <c r="A266" s="19" t="s">
-        <v>3</v>
+      <c r="A266" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="B266" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="C266" s="31" t="s">
-        <v>1975</v>
-      </c>
-      <c r="D266" s="38"/>
+        <v>295</v>
+      </c>
+      <c r="C266" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="D266" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="267" spans="1:4" ht="15" customHeight="1">
       <c r="A267" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B267" s="18" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C267" s="31" t="s">
-        <v>1976</v>
-      </c>
-      <c r="D267" s="38"/>
+        <v>1972</v>
+      </c>
+      <c r="D267" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="268" spans="1:4" ht="15" customHeight="1">
-      <c r="A268" s="19" t="s">
-        <v>3</v>
+      <c r="A268" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="B268" s="18" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C268" s="31" t="s">
-        <v>1977</v>
-      </c>
-      <c r="D268" s="38"/>
+        <v>1973</v>
+      </c>
+      <c r="D268" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="269" spans="1:4" ht="15" customHeight="1">
       <c r="A269" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B269" s="18" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C269" s="31" t="s">
-        <v>1978</v>
-      </c>
-      <c r="D269" s="38"/>
+        <v>1974</v>
+      </c>
+      <c r="D269" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="270" spans="1:4" ht="15" customHeight="1">
-      <c r="A270" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B270" s="30" t="s">
-        <v>303</v>
-      </c>
-      <c r="C270" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="D270" s="38" t="s">
-        <v>894</v>
-      </c>
+      <c r="A270" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B270" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C270" s="31" t="s">
+        <v>1975</v>
+      </c>
+      <c r="D270" s="38"/>
     </row>
     <row r="271" spans="1:4" ht="15" customHeight="1">
       <c r="A271" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B271" s="18" t="s">
-        <v>1843</v>
+        <v>300</v>
       </c>
       <c r="C271" s="31" t="s">
-        <v>1844</v>
-      </c>
-      <c r="D271" s="38" t="s">
-        <v>894</v>
-      </c>
+        <v>1976</v>
+      </c>
+      <c r="D271" s="38"/>
     </row>
     <row r="272" spans="1:4" ht="15" customHeight="1">
       <c r="A272" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B272" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="C272" s="9" t="s">
-        <v>306</v>
+        <v>301</v>
+      </c>
+      <c r="C272" s="31" t="s">
+        <v>1977</v>
       </c>
       <c r="D272" s="38"/>
     </row>
@@ -31569,90 +31837,88 @@
         <v>1</v>
       </c>
       <c r="B273" s="18" t="s">
-        <v>307</v>
-      </c>
-      <c r="C273" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="D273" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="C273" s="31" t="s">
+        <v>1978</v>
+      </c>
+      <c r="D273" s="38"/>
+    </row>
+    <row r="274" spans="1:4" ht="15" customHeight="1">
+      <c r="A274" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B274" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="C274" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="D274" s="38" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="274" spans="1:4" ht="15" customHeight="1">
-      <c r="A274" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B274" s="18" t="s">
-        <v>309</v>
-      </c>
-      <c r="C274" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="D274" s="38"/>
     </row>
     <row r="275" spans="1:4" ht="15" customHeight="1">
       <c r="A275" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B275" s="24" t="s">
-        <v>1547</v>
-      </c>
-      <c r="C275" s="9" t="s">
-        <v>308</v>
+      <c r="B275" s="18" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C275" s="31" t="s">
+        <v>1844</v>
       </c>
       <c r="D275" s="38" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="15" customHeight="1">
-      <c r="A276" s="8" t="s">
-        <v>1</v>
+      <c r="A276" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="B276" s="18" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="D276" s="38" t="s">
-        <v>894</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="D276" s="38"/>
     </row>
     <row r="277" spans="1:4" ht="15" customHeight="1">
       <c r="A277" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B277" s="18" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="D277" s="38"/>
+        <v>308</v>
+      </c>
+      <c r="D277" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="278" spans="1:4" ht="15" customHeight="1">
-      <c r="A278" s="8" t="s">
-        <v>1</v>
+      <c r="A278" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="B278" s="18" t="s">
-        <v>1769</v>
+        <v>309</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>1770</v>
-      </c>
-      <c r="D278" s="38" t="s">
-        <v>894</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="D278" s="38"/>
     </row>
     <row r="279" spans="1:4" ht="15" customHeight="1">
       <c r="A279" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B279" s="18" t="s">
-        <v>1772</v>
+      <c r="B279" s="24" t="s">
+        <v>1547</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>1771</v>
+        <v>308</v>
       </c>
       <c r="D279" s="38" t="s">
         <v>894</v>
@@ -31663,13 +31929,13 @@
         <v>1</v>
       </c>
       <c r="B280" s="18" t="s">
-        <v>1850</v>
-      </c>
-      <c r="C280" s="31" t="s">
-        <v>1853</v>
+        <v>311</v>
+      </c>
+      <c r="C280" s="9" t="s">
+        <v>312</v>
       </c>
       <c r="D280" s="38" t="s">
-        <v>1851</v>
+        <v>894</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="15" customHeight="1">
@@ -31677,72 +31943,78 @@
         <v>1</v>
       </c>
       <c r="B281" s="18" t="s">
-        <v>1855</v>
-      </c>
-      <c r="C281" s="31" t="s">
-        <v>1854</v>
-      </c>
-      <c r="D281" s="38" t="s">
-        <v>1851</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="C281" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D281" s="38"/>
     </row>
     <row r="282" spans="1:4" ht="15" customHeight="1">
       <c r="A282" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B282" s="18" t="s">
-        <v>1773</v>
+        <v>1769</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D282" s="38"/>
+        <v>1770</v>
+      </c>
+      <c r="D282" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="283" spans="1:4" ht="15" customHeight="1">
       <c r="A283" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B283" s="18" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>1776</v>
-      </c>
-      <c r="D283" s="38"/>
+        <v>1771</v>
+      </c>
+      <c r="D283" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="284" spans="1:4" ht="15" customHeight="1">
       <c r="A284" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B284" s="18" t="s">
-        <v>1885</v>
-      </c>
-      <c r="C284" s="9" t="s">
-        <v>1884</v>
-      </c>
-      <c r="D284" s="38"/>
+        <v>1850</v>
+      </c>
+      <c r="C284" s="31" t="s">
+        <v>1853</v>
+      </c>
+      <c r="D284" s="38" t="s">
+        <v>1851</v>
+      </c>
     </row>
     <row r="285" spans="1:4" ht="15" customHeight="1">
       <c r="A285" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B285" s="18" t="s">
-        <v>315</v>
-      </c>
-      <c r="C285" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="D285" s="38"/>
+        <v>1855</v>
+      </c>
+      <c r="C285" s="31" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D285" s="38" t="s">
+        <v>1851</v>
+      </c>
     </row>
     <row r="286" spans="1:4" ht="15" customHeight="1">
       <c r="A286" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B286" s="18" t="s">
-        <v>317</v>
-      </c>
-      <c r="C286" s="10" t="s">
-        <v>387</v>
+        <v>1773</v>
+      </c>
+      <c r="C286" s="9" t="s">
+        <v>1774</v>
       </c>
       <c r="D286" s="38"/>
     </row>
@@ -31751,10 +32023,10 @@
         <v>1</v>
       </c>
       <c r="B287" s="18" t="s">
-        <v>922</v>
-      </c>
-      <c r="C287" s="10" t="s">
-        <v>810</v>
+        <v>1775</v>
+      </c>
+      <c r="C287" s="9" t="s">
+        <v>1776</v>
       </c>
       <c r="D287" s="38"/>
     </row>
@@ -31763,38 +32035,46 @@
         <v>1</v>
       </c>
       <c r="B288" s="18" t="s">
-        <v>1858</v>
-      </c>
-      <c r="C288" s="10" t="s">
-        <v>1859</v>
+        <v>1885</v>
+      </c>
+      <c r="C288" s="9" t="s">
+        <v>1884</v>
       </c>
       <c r="D288" s="38"/>
     </row>
-    <row r="289" spans="1:4">
-      <c r="A289" s="2"/>
-      <c r="B289" s="2"/>
-      <c r="C289" s="2"/>
-      <c r="D289" s="44"/>
+    <row r="289" spans="1:4" ht="15" customHeight="1">
+      <c r="A289" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B289" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="C289" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D289" s="38"/>
     </row>
     <row r="290" spans="1:4" ht="15" customHeight="1">
-      <c r="A290" s="25" t="s">
-        <v>853</v>
-      </c>
-      <c r="B290" s="26"/>
-      <c r="C290" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="D290" s="44"/>
+      <c r="A290" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B290" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="C290" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D290" s="38"/>
     </row>
     <row r="291" spans="1:4" ht="15" customHeight="1">
-      <c r="A291" s="6" t="s">
+      <c r="A291" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B291" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="C291" s="7" t="s">
-        <v>269</v>
+      <c r="B291" s="18" t="s">
+        <v>922</v>
+      </c>
+      <c r="C291" s="10" t="s">
+        <v>810</v>
       </c>
       <c r="D291" s="38"/>
     </row>
@@ -31802,67 +32082,51 @@
       <c r="A292" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B292" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="C292" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="D292" s="38" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4" ht="15" customHeight="1">
-      <c r="A293" s="8" t="s">
+      <c r="B292" s="18" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C292" s="10" t="s">
+        <v>1859</v>
+      </c>
+      <c r="D292" s="38"/>
+    </row>
+    <row r="293" spans="1:4">
+      <c r="A293" s="2"/>
+      <c r="B293" s="2"/>
+      <c r="C293" s="2"/>
+      <c r="D293" s="44"/>
+    </row>
+    <row r="294" spans="1:4" ht="15" customHeight="1">
+      <c r="A294" s="25" t="s">
+        <v>853</v>
+      </c>
+      <c r="B294" s="26"/>
+      <c r="C294" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D294" s="44"/>
+    </row>
+    <row r="295" spans="1:4" ht="15" customHeight="1">
+      <c r="A295" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B293" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="C293" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="D293" s="38" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="294" spans="1:4" ht="15" customHeight="1">
-      <c r="A294" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B294" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="C294" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="D294" s="38" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="295" spans="1:4" ht="15" customHeight="1">
-      <c r="A295" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B295" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="C295" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="D295" s="38" t="s">
-        <v>894</v>
-      </c>
+      <c r="B295" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="C295" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D295" s="38"/>
     </row>
     <row r="296" spans="1:4" ht="15" customHeight="1">
       <c r="A296" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B296" s="18" t="s">
-        <v>274</v>
+      <c r="B296" s="30" t="s">
+        <v>270</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D296" s="38" t="s">
         <v>894</v>
@@ -31873,133 +32137,133 @@
         <v>1</v>
       </c>
       <c r="B297" s="18" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="D297" s="38"/>
+        <v>280</v>
+      </c>
+      <c r="D297" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="298" spans="1:4" ht="15" customHeight="1">
       <c r="A298" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B298" s="18" t="s">
-        <v>277</v>
+      <c r="B298" s="30" t="s">
+        <v>272</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D298" s="38" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="299" spans="1:4">
-      <c r="D299" s="44"/>
+    <row r="299" spans="1:4" ht="15" customHeight="1">
+      <c r="A299" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B299" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C299" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="D299" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="300" spans="1:4" ht="15" customHeight="1">
-      <c r="A300" s="27" t="s">
-        <v>854</v>
-      </c>
-      <c r="B300" s="26"/>
-      <c r="C300" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="D300" s="44"/>
+      <c r="A300" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B300" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C300" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D300" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="301" spans="1:4" ht="15" customHeight="1">
-      <c r="A301" s="6" t="s">
+      <c r="A301" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B301" s="23" t="s">
-        <v>1947</v>
-      </c>
-      <c r="C301" s="7" t="s">
-        <v>1943</v>
-      </c>
-      <c r="D301" s="38" t="s">
-        <v>894</v>
-      </c>
+      <c r="B301" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C301" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D301" s="38"/>
     </row>
     <row r="302" spans="1:4" ht="15" customHeight="1">
-      <c r="A302" s="6" t="s">
+      <c r="A302" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B302" s="23" t="s">
-        <v>1948</v>
-      </c>
-      <c r="C302" s="7" t="s">
-        <v>1945</v>
+      <c r="B302" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C302" s="9" t="s">
+        <v>278</v>
       </c>
       <c r="D302" s="38" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="303" spans="1:4" ht="15" customHeight="1">
-      <c r="A303" s="6" t="s">
+    <row r="303" spans="1:4">
+      <c r="D303" s="44"/>
+    </row>
+    <row r="304" spans="1:4" ht="15" customHeight="1">
+      <c r="A304" s="27" t="s">
+        <v>854</v>
+      </c>
+      <c r="B304" s="26"/>
+      <c r="C304" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="D304" s="44"/>
+    </row>
+    <row r="305" spans="1:4" ht="15" customHeight="1">
+      <c r="A305" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B303" s="23" t="s">
-        <v>753</v>
-      </c>
-      <c r="C303" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="D303" s="38" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="304" spans="1:4" ht="15" customHeight="1">
-      <c r="A304" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B304" s="24" t="s">
-        <v>754</v>
-      </c>
-      <c r="C304" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="D304" s="38" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="305" spans="1:4" ht="15" customHeight="1">
-      <c r="A305" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B305" s="24" t="s">
-        <v>755</v>
-      </c>
-      <c r="C305" s="9" t="s">
-        <v>260</v>
+      <c r="B305" s="23" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C305" s="7" t="s">
+        <v>1943</v>
       </c>
       <c r="D305" s="38" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="15" customHeight="1">
-      <c r="A306" s="8" t="s">
+      <c r="A306" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B306" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="C306" s="9" t="s">
-        <v>262</v>
+      <c r="B306" s="23" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C306" s="7" t="s">
+        <v>1945</v>
       </c>
       <c r="D306" s="38" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="15" customHeight="1">
-      <c r="A307" s="8" t="s">
+      <c r="A307" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B307" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="C307" s="9" t="s">
-        <v>264</v>
+      <c r="B307" s="23" t="s">
+        <v>753</v>
+      </c>
+      <c r="C307" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="D307" s="38" t="s">
         <v>894</v>
@@ -32009,23 +32273,25 @@
       <c r="A308" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B308" s="18" t="s">
-        <v>265</v>
+      <c r="B308" s="24" t="s">
+        <v>754</v>
       </c>
       <c r="C308" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="D308" s="38"/>
+        <v>259</v>
+      </c>
+      <c r="D308" s="38" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="309" spans="1:4" ht="15" customHeight="1">
       <c r="A309" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B309" s="18" t="s">
-        <v>267</v>
+      <c r="B309" s="24" t="s">
+        <v>755</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>710</v>
+        <v>260</v>
       </c>
       <c r="D309" s="38" t="s">
         <v>894</v>
@@ -32036,10 +32302,10 @@
         <v>1</v>
       </c>
       <c r="B310" s="18" t="s">
-        <v>738</v>
+        <v>261</v>
       </c>
       <c r="C310" s="9" t="s">
-        <v>711</v>
+        <v>262</v>
       </c>
       <c r="D310" s="38" t="s">
         <v>894</v>
@@ -32050,10 +32316,10 @@
         <v>1</v>
       </c>
       <c r="B311" s="18" t="s">
-        <v>740</v>
+        <v>263</v>
       </c>
       <c r="C311" s="9" t="s">
-        <v>713</v>
+        <v>264</v>
       </c>
       <c r="D311" s="38" t="s">
         <v>894</v>
@@ -32064,24 +32330,22 @@
         <v>1</v>
       </c>
       <c r="B312" s="18" t="s">
-        <v>741</v>
+        <v>265</v>
       </c>
       <c r="C312" s="9" t="s">
-        <v>712</v>
-      </c>
-      <c r="D312" s="38" t="s">
-        <v>894</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="D312" s="38"/>
     </row>
     <row r="313" spans="1:4" ht="15" customHeight="1">
       <c r="A313" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B313" s="18" t="s">
-        <v>742</v>
+        <v>267</v>
       </c>
       <c r="C313" s="9" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="D313" s="38" t="s">
         <v>894</v>
@@ -32092,10 +32356,10 @@
         <v>1</v>
       </c>
       <c r="B314" s="18" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="C314" s="9" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="D314" s="38" t="s">
         <v>894</v>
@@ -32106,10 +32370,10 @@
         <v>1</v>
       </c>
       <c r="B315" s="18" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="C315" s="9" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="D315" s="38" t="s">
         <v>894</v>
@@ -32120,10 +32384,10 @@
         <v>1</v>
       </c>
       <c r="B316" s="18" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="C316" s="9" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="D316" s="38" t="s">
         <v>894</v>
@@ -32134,10 +32398,10 @@
         <v>1</v>
       </c>
       <c r="B317" s="18" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="C317" s="9" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="D317" s="38" t="s">
         <v>894</v>
@@ -32148,10 +32412,10 @@
         <v>1</v>
       </c>
       <c r="B318" s="18" t="s">
-        <v>752</v>
+        <v>743</v>
       </c>
       <c r="C318" s="9" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="D318" s="38" t="s">
         <v>894</v>
@@ -32162,10 +32426,10 @@
         <v>1</v>
       </c>
       <c r="B319" s="18" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="C319" s="9" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D319" s="38" t="s">
         <v>894</v>
@@ -32176,12 +32440,68 @@
         <v>1</v>
       </c>
       <c r="B320" s="18" t="s">
+        <v>746</v>
+      </c>
+      <c r="C320" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="D320" s="38" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" ht="15" customHeight="1">
+      <c r="A321" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B321" s="18" t="s">
+        <v>748</v>
+      </c>
+      <c r="C321" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="D321" s="38" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" ht="15" customHeight="1">
+      <c r="A322" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B322" s="18" t="s">
+        <v>752</v>
+      </c>
+      <c r="C322" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D322" s="38" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" ht="15" customHeight="1">
+      <c r="A323" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B323" s="18" t="s">
+        <v>750</v>
+      </c>
+      <c r="C323" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="D323" s="38" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" ht="15" customHeight="1">
+      <c r="A324" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B324" s="18" t="s">
         <v>749</v>
       </c>
-      <c r="C320" s="9" t="s">
+      <c r="C324" s="9" t="s">
         <v>723</v>
       </c>
-      <c r="D320" s="38" t="s">
+      <c r="D324" s="38" t="s">
         <v>894</v>
       </c>
     </row>
@@ -32208,9 +32528,9 @@
     <hyperlink ref="C129" r:id="rId3" display="https://github.com/mYmd/VBA/blob/master/Haskell_3_printM.bas"/>
     <hyperlink ref="C135" r:id="rId4" display="https://github.com/mYmd/VBA/blob/master/Haskell_4_vector.bas"/>
     <hyperlink ref="C188" r:id="rId5" display="https://github.com/mYmd/VBA/blob/master/Haskell_5_sort.bas"/>
-    <hyperlink ref="C300" r:id="rId6" display="https://github.com/mYmd/VBA/blob/master/misc_math.bas"/>
-    <hyperlink ref="C290" r:id="rId7" display="https://github.com/mYmd/VBA/blob/master/misc_random.bas"/>
-    <hyperlink ref="C246" r:id="rId8" display="https://github.com/mYmd/VBA/blob/master/misc_utility"/>
+    <hyperlink ref="C304" r:id="rId6" display="https://github.com/mYmd/VBA/blob/master/misc_math.bas"/>
+    <hyperlink ref="C294" r:id="rId7" display="https://github.com/mYmd/VBA/blob/master/misc_random.bas"/>
+    <hyperlink ref="C250" r:id="rId8" display="https://github.com/mYmd/VBA/blob/master/misc_utility"/>
     <hyperlink ref="B26" location="_moveVariant" display="moveVariant"/>
     <hyperlink ref="B27" location="_ph_0" display="ph_0"/>
     <hyperlink ref="B28" location="_ph_1" display="ph_1"/>
@@ -32361,142 +32681,146 @@
     <hyperlink ref="B198" location="_equal_range_pred" display="_equal_range_pred"/>
     <hyperlink ref="B199" location="_partition_points" display="_partition_points"/>
     <hyperlink ref="B200" location="_partition_points_pred" display="_partition_points_pred"/>
-    <hyperlink ref="B303" location="_sin_fun" display="_sin_fun"/>
-    <hyperlink ref="B304" location="_cos_fun" display="_cos_fun"/>
-    <hyperlink ref="B305" location="_pow_fun" display="_pow_fun"/>
-    <hyperlink ref="B306" location="_make_polyCoef" display="_make_polyCoef"/>
-    <hyperlink ref="B307" location="_newton_method" display="_newton_method"/>
-    <hyperlink ref="B308" location="_integral_simpson" display="_integral_simpson"/>
-    <hyperlink ref="B309" location="_make_complex" display="_make_complex"/>
-    <hyperlink ref="B310" location="_make_complex_polar" display="_make_complex_polar"/>
-    <hyperlink ref="B311" location="_show_complex" display="_show_complex"/>
-    <hyperlink ref="B312" location="_show_complex_polar" display="_show_complex_polar"/>
-    <hyperlink ref="B320" location="_complex_arg" display="_complex_arg"/>
-    <hyperlink ref="B319" location="_complex_abs" display="_complex_abs"/>
-    <hyperlink ref="B318" location="_complex_abs2" display="_complex_abs2"/>
-    <hyperlink ref="B317" location="_complex_cnj" display="_complex_cnj"/>
-    <hyperlink ref="B316" location="_complex_divide" display="_complex_divide"/>
-    <hyperlink ref="B315" location="_complex_mult" display="_complex_mult"/>
-    <hyperlink ref="B314" location="_complex_minus" display="_complex_minus"/>
-    <hyperlink ref="B313" location="_complex_add" display="_complex_add"/>
-    <hyperlink ref="B291" location="_seed_Engine" display="_seed_Engine"/>
-    <hyperlink ref="B292" location="_uniform_int_dist" display="_uniform_int_dist"/>
-    <hyperlink ref="B293" location="_uniform_real_dist" display="_uniform_real_dist"/>
-    <hyperlink ref="B294" location="_normal_dist" display="_normal_dist"/>
-    <hyperlink ref="B295" location="_bernoulli_dist" display="_bernoulli_dist"/>
-    <hyperlink ref="B296" location="_discrete_dist" display="_discrete_dist"/>
-    <hyperlink ref="B297" location="_random_iota" display="_random_iota"/>
-    <hyperlink ref="B298" location="_random_shuffle" display="_random_shuffle"/>
-    <hyperlink ref="B247" location="_p__n" display="_p__n"/>
-    <hyperlink ref="B251" location="_p_typename" display="_p_typename"/>
-    <hyperlink ref="B253" location="_p_format" display="_p_format"/>
-    <hyperlink ref="B254" location="_p_InStr" display="_p_InStr"/>
-    <hyperlink ref="B255" location="_p_InStrRev" display="_p_InStrRev"/>
-    <hyperlink ref="B259" location="_separate_string" display="_separate_string"/>
+    <hyperlink ref="B307" location="_sin_fun" display="_sin_fun"/>
+    <hyperlink ref="B308" location="_cos_fun" display="_cos_fun"/>
+    <hyperlink ref="B309" location="_pow_fun" display="_pow_fun"/>
+    <hyperlink ref="B310" location="_make_polyCoef" display="_make_polyCoef"/>
+    <hyperlink ref="B311" location="_newton_method" display="_newton_method"/>
+    <hyperlink ref="B312" location="_integral_simpson" display="_integral_simpson"/>
+    <hyperlink ref="B313" location="_make_complex" display="_make_complex"/>
+    <hyperlink ref="B314" location="_make_complex_polar" display="_make_complex_polar"/>
+    <hyperlink ref="B315" location="_show_complex" display="_show_complex"/>
+    <hyperlink ref="B316" location="_show_complex_polar" display="_show_complex_polar"/>
+    <hyperlink ref="B324" location="_complex_arg" display="_complex_arg"/>
+    <hyperlink ref="B323" location="_complex_abs" display="_complex_abs"/>
+    <hyperlink ref="B322" location="_complex_abs2" display="_complex_abs2"/>
+    <hyperlink ref="B321" location="_complex_cnj" display="_complex_cnj"/>
+    <hyperlink ref="B320" location="_complex_divide" display="_complex_divide"/>
+    <hyperlink ref="B319" location="_complex_mult" display="_complex_mult"/>
+    <hyperlink ref="B318" location="_complex_minus" display="_complex_minus"/>
+    <hyperlink ref="B317" location="_complex_add" display="_complex_add"/>
+    <hyperlink ref="B295" location="_seed_Engine" display="_seed_Engine"/>
+    <hyperlink ref="B296" location="_uniform_int_dist" display="_uniform_int_dist"/>
+    <hyperlink ref="B297" location="_uniform_real_dist" display="_uniform_real_dist"/>
+    <hyperlink ref="B298" location="_normal_dist" display="_normal_dist"/>
+    <hyperlink ref="B299" location="_bernoulli_dist" display="_bernoulli_dist"/>
+    <hyperlink ref="B300" location="_discrete_dist" display="_discrete_dist"/>
+    <hyperlink ref="B301" location="_random_iota" display="_random_iota"/>
+    <hyperlink ref="B302" location="_random_shuffle" display="_random_shuffle"/>
+    <hyperlink ref="B251" location="_p__n" display="_p__n"/>
+    <hyperlink ref="B255" location="_p_typename" display="_p_typename"/>
+    <hyperlink ref="B257" location="_p_format" display="_p_format"/>
+    <hyperlink ref="B258" location="_p_InStr" display="_p_InStr"/>
+    <hyperlink ref="B259" location="_p_InStrRev" display="_p_InStrRev"/>
+    <hyperlink ref="B263" location="_separate_string" display="_separate_string"/>
     <hyperlink ref="B59" location="_p_foldl1" display="_p_foldl1"/>
     <hyperlink ref="B60" location="_p_foldr1" display="_p_foldr1"/>
     <hyperlink ref="B63" location="_p_scanl1" display="_p_scanl1"/>
     <hyperlink ref="B64" location="_p_scanr1" display="_p_scanr1"/>
-    <hyperlink ref="B260" location="_subM_R" display="_subM_R"/>
-    <hyperlink ref="B261" location="_subM_R_b" display="_subM_R_b"/>
-    <hyperlink ref="B262" location="_subM_C" display="_subM_C"/>
-    <hyperlink ref="B263" location="_subM_C_b" display="_subM_C_b"/>
-    <hyperlink ref="B264" location="_selectRow_b" display="_selectRow_b"/>
-    <hyperlink ref="B265" location="_selectCol_b" display="_selectCol_b"/>
-    <hyperlink ref="B266" location="_fillRow_b" display="_fillRow_b"/>
-    <hyperlink ref="B267" location="_fillRow_b_move" display="_fillRow_b_move"/>
-    <hyperlink ref="B268" location="_fillCol_b" display="_fillCol_b"/>
-    <hyperlink ref="B269" location="_fillCol_b_move" display="_fillCol_b_move"/>
-    <hyperlink ref="B272" location="_rowWise_change" display="_rowWise_change"/>
-    <hyperlink ref="B273" location="_rowWise_change_move" display="_rowWise_change_move"/>
-    <hyperlink ref="B274" location="_columnWise_change" display="_columnWise_change"/>
-    <hyperlink ref="B286" location="_group_by_partition_points" display="_group_by_partition_points"/>
-    <hyperlink ref="B285" location="_splitStr2Funs" display="_splitStr2Funs"/>
-    <hyperlink ref="B277" location="_equal_all_pred" display="_equal_all_pred"/>
-    <hyperlink ref="B276" location="_equal_all" display="_equal_all"/>
-    <hyperlink ref="B275" location="_columnWise_change_move" display="_columnWise_change_move"/>
-    <hyperlink ref="B248" location="_p_try" display="_p_try"/>
-    <hyperlink ref="B270" location="_adjacent_op" display="_adjacent_op"/>
+    <hyperlink ref="B264" location="_subM_R" display="_subM_R"/>
+    <hyperlink ref="B265" location="_subM_R_b" display="_subM_R_b"/>
+    <hyperlink ref="B266" location="_subM_C" display="_subM_C"/>
+    <hyperlink ref="B267" location="_subM_C_b" display="_subM_C_b"/>
+    <hyperlink ref="B268" location="_selectRow_b" display="_selectRow_b"/>
+    <hyperlink ref="B269" location="_selectCol_b" display="_selectCol_b"/>
+    <hyperlink ref="B270" location="_fillRow_b" display="_fillRow_b"/>
+    <hyperlink ref="B271" location="_fillRow_b_move" display="_fillRow_b_move"/>
+    <hyperlink ref="B272" location="_fillCol_b" display="_fillCol_b"/>
+    <hyperlink ref="B273" location="_fillCol_b_move" display="_fillCol_b_move"/>
+    <hyperlink ref="B276" location="_rowWise_change" display="_rowWise_change"/>
+    <hyperlink ref="B277" location="_rowWise_change_move" display="_rowWise_change_move"/>
+    <hyperlink ref="B278" location="_columnWise_change" display="_columnWise_change"/>
+    <hyperlink ref="B290" location="_group_by_partition_points" display="_group_by_partition_points"/>
+    <hyperlink ref="B289" location="_splitStr2Funs" display="_splitStr2Funs"/>
+    <hyperlink ref="B281" location="_equal_all_pred" display="_equal_all_pred"/>
+    <hyperlink ref="B280" location="_equal_all" display="_equal_all"/>
+    <hyperlink ref="B279" location="_columnWise_change_move" display="_columnWise_change_move"/>
+    <hyperlink ref="B252" location="_p_try" display="_p_try"/>
+    <hyperlink ref="B274" location="_adjacent_op" display="_adjacent_op"/>
     <hyperlink ref="B7" location="_mapF_imple" display="_mapF_imple"/>
     <hyperlink ref="B17" location="_stdsort" display="_stdsort"/>
     <hyperlink ref="B19" location="_find_best_imple" display="find_best_imple"/>
     <hyperlink ref="B20" location="_repeat_imple" display="_repeat_imple"/>
-    <hyperlink ref="B249" location="_p_try_not" display="_p_try_not"/>
+    <hyperlink ref="B253" location="_p_try_not" display="_p_try_not"/>
     <hyperlink ref="B201" location="_less_dic" display="_less_dic"/>
     <hyperlink ref="B202" location="_less_equal_dic" display="_less_equal_dic"/>
     <hyperlink ref="B203" location="_greater_dic" display="_greater_dic"/>
     <hyperlink ref="B204" location="_greater_equal_dic" display="_greater_equal_dic"/>
     <hyperlink ref="B1" location="_files" display="ファイル構成"/>
-    <hyperlink ref="B250" location="_p_try_less" display="_p_try_less"/>
-    <hyperlink ref="B252" location="_p_isNumeric" display="_p_isNumeric"/>
-    <hyperlink ref="B257" location="_p_StrConv" display="_p_StrConv"/>
-    <hyperlink ref="B209" location="_New_vh_stdvec" display="New"/>
-    <hyperlink ref="B210" location="_from_vh_stdvec" display="from"/>
-    <hyperlink ref="B211" location="_clear" display="_clear"/>
-    <hyperlink ref="B212" location="_free" display="_free"/>
-    <hyperlink ref="B215" location="_size" display="_size"/>
-    <hyperlink ref="B216" location="_capacity" display="_capacity"/>
-    <hyperlink ref="B217" location="_shrink" display="_shrink"/>
-    <hyperlink ref="B218" location="_erase_n" display="_erase_n"/>
-    <hyperlink ref="B219" location="_vec_printS" display="printS"/>
-    <hyperlink ref="B220" location="_vec_printM" display="_vec_printM"/>
-    <hyperlink ref="B221" location="_vec_printM_" display="_vec_printM_"/>
-    <hyperlink ref="B222" location="_val" display="_val"/>
-    <hyperlink ref="B223" location="_pop" display="_pop"/>
-    <hyperlink ref="B224" location="_push" display="_push"/>
-    <hyperlink ref="B225" location="_push_n" display="_push_n"/>
-    <hyperlink ref="B226" location="_push_array" display="_push_array"/>
-    <hyperlink ref="B213" location="_swap_vh_stdvec" display="swap"/>
-    <hyperlink ref="B227" location="_insert_empty" display="_insert_empty"/>
-    <hyperlink ref="B228" location="_push_back" display="_push_back"/>
-    <hyperlink ref="B229" location="_push_back_n" display="_push_back_n"/>
-    <hyperlink ref="B230" location="_push_back_array" display="_push_back_array"/>
+    <hyperlink ref="B254" location="_p_try_less" display="_p_try_less"/>
+    <hyperlink ref="B256" location="_p_isNumeric" display="_p_isNumeric"/>
+    <hyperlink ref="B261" location="_p_StrConv" display="_p_StrConv"/>
+    <hyperlink ref="B213" location="_New_vh_stdvec" display="New"/>
+    <hyperlink ref="B214" location="_from_vh_stdvec" display="from"/>
+    <hyperlink ref="B215" location="_clear" display="_clear"/>
+    <hyperlink ref="B216" location="_free" display="_free"/>
+    <hyperlink ref="B219" location="_size" display="_size"/>
+    <hyperlink ref="B220" location="_capacity" display="_capacity"/>
+    <hyperlink ref="B221" location="_shrink" display="_shrink"/>
+    <hyperlink ref="B222" location="_erase_n" display="_erase_n"/>
+    <hyperlink ref="B223" location="_vec_printS" display="printS"/>
+    <hyperlink ref="B224" location="_vec_printM" display="_vec_printM"/>
+    <hyperlink ref="B225" location="_vec_printM_" display="_vec_printM_"/>
+    <hyperlink ref="B226" location="_val" display="_val"/>
+    <hyperlink ref="B227" location="_pop" display="_pop"/>
+    <hyperlink ref="B228" location="_push" display="_push"/>
+    <hyperlink ref="B229" location="_push_n" display="_push_n"/>
+    <hyperlink ref="B230" location="_push_array" display="_push_array"/>
+    <hyperlink ref="B217" location="_swap_vh_stdvec" display="swap"/>
+    <hyperlink ref="B231" location="_insert_empty" display="_insert_empty"/>
+    <hyperlink ref="B232" location="_push_back" display="_push_back"/>
+    <hyperlink ref="B233" location="_push_back_n" display="_push_back_n"/>
+    <hyperlink ref="B234" location="_push_back_array" display="_push_back_array"/>
     <hyperlink ref="C2" r:id="rId9" display="https://github.com/mYmd/VBA/blob/master/Haskell_0_declare.bas"/>
     <hyperlink ref="C1" r:id="rId10"/>
-    <hyperlink ref="B214" location="_clone_vh_stdvec" display="clone"/>
-    <hyperlink ref="B234" location="_orderby_vh_stdvec" display="orderby"/>
-    <hyperlink ref="B233" location="_map_vh_stdvec" display="map"/>
-    <hyperlink ref="B232" location="_filter_vh_stdvec" display="filter"/>
-    <hyperlink ref="B278" location="_filter_if" display="filter_if"/>
-    <hyperlink ref="B279" location="_filter_if_not" display="filter_if_not"/>
-    <hyperlink ref="B282" location="_2pipe" display="pipe"/>
-    <hyperlink ref="B283" location="_2pipe_" display="pipe_"/>
-    <hyperlink ref="B237" location="_pipe" display="pipe"/>
-    <hyperlink ref="B238" location="_pipe_" display="pipe_"/>
-    <hyperlink ref="B239" location="_pipe_X" display="x"/>
-    <hyperlink ref="B240" location="_pipe_arrow" display="→"/>
-    <hyperlink ref="B241" location="_pipe_val" display="val"/>
-    <hyperlink ref="B242" location="_pipe_pop" display="pop"/>
-    <hyperlink ref="B243" location="_pipe_swap" display="swap"/>
-    <hyperlink ref="B244" location="_pipe_clone" display="clone"/>
+    <hyperlink ref="B218" location="_clone_vh_stdvec" display="clone"/>
+    <hyperlink ref="B238" location="_orderby_vh_stdvec" display="orderby"/>
+    <hyperlink ref="B237" location="_map_vh_stdvec" display="map"/>
+    <hyperlink ref="B236" location="_filter_vh_stdvec" display="filter"/>
+    <hyperlink ref="B282" location="_filter_if" display="filter_if"/>
+    <hyperlink ref="B283" location="_filter_if_not" display="filter_if_not"/>
+    <hyperlink ref="B286" location="_2pipe" display="pipe"/>
+    <hyperlink ref="B287" location="_2pipe_" display="pipe_"/>
+    <hyperlink ref="B241" location="_pipe" display="pipe"/>
+    <hyperlink ref="B242" location="_pipe_" display="pipe_"/>
+    <hyperlink ref="B243" location="_pipe_X" display="x"/>
+    <hyperlink ref="B244" location="_pipe_arrow" display="→"/>
+    <hyperlink ref="B245" location="_pipe_val" display="val"/>
+    <hyperlink ref="B246" location="_pipe_pop" display="pop"/>
+    <hyperlink ref="B247" location="_pipe_swap" display="swap"/>
+    <hyperlink ref="B248" location="_pipe_clone" display="clone"/>
     <hyperlink ref="B23" location="_self_zipWith" display="self_zipWith"/>
-    <hyperlink ref="B258" location="_p_Trim" display="p_Trim"/>
-    <hyperlink ref="B271" location="_get_unique" display="get_unique"/>
-    <hyperlink ref="B280" location="_p_Not" display="p_Not"/>
-    <hyperlink ref="B281" location="_p_imply" display="p_imply"/>
-    <hyperlink ref="B287" location="_csv2Vector" display="_csv2Vector"/>
-    <hyperlink ref="B288" location="_A_overlap_B" display="A_overlap_B"/>
+    <hyperlink ref="B262" location="_p_Trim" display="p_Trim"/>
+    <hyperlink ref="B275" location="_get_unique" display="get_unique"/>
+    <hyperlink ref="B284" location="_p_Not" display="p_Not"/>
+    <hyperlink ref="B285" location="_p_imply" display="p_imply"/>
+    <hyperlink ref="B291" location="_csv2Vector" display="_csv2Vector"/>
+    <hyperlink ref="B292" location="_A_overlap_B" display="A_overlap_B"/>
     <hyperlink ref="B205" location="_equal_dic" display="equal_dic"/>
     <hyperlink ref="B206" location="_notEqual_dic" display="notEqual_dic"/>
-    <hyperlink ref="B284" location="____stdVec" display="stdVec"/>
+    <hyperlink ref="B288" location="____stdVec" display="stdVec"/>
     <hyperlink ref="B57" location="_p_foldl" display="p_foldl"/>
     <hyperlink ref="B58" location="_p_foldr" display="p_foldr"/>
     <hyperlink ref="B61" location="_p_scanl" display="p_scanl"/>
     <hyperlink ref="B62" location="_p_scanr" display="p_scanr"/>
-    <hyperlink ref="B256" location="_p_Like" display="p_Like"/>
+    <hyperlink ref="B260" location="_p_Like" display="p_Like"/>
     <hyperlink ref="B183" location="__push_back" display="push_back"/>
     <hyperlink ref="B184" location="_push_back_move" display="push_back_move"/>
     <hyperlink ref="B185" location="_flatten" display="flatten"/>
-    <hyperlink ref="B301" location="_isPrimeNumber" display="isPrimeNumber"/>
-    <hyperlink ref="B302" location="_primeNumbers" display="primeNumbers"/>
+    <hyperlink ref="B305" location="_isPrimeNumber" display="isPrimeNumber"/>
+    <hyperlink ref="B306" location="_primeNumbers" display="primeNumbers"/>
     <hyperlink ref="B86" location="_place_fill" display="place_fill"/>
     <hyperlink ref="B78" location="_firstArg" display="p_identity"/>
     <hyperlink ref="B75" location="_assignVar" display="assignVar"/>
     <hyperlink ref="B96" location="_maskVar" display="maskVar"/>
     <hyperlink ref="B169" location="_catVs_move" display="catV_move"/>
     <hyperlink ref="B171" location="_catVs_move" display="catVs_move"/>
-    <hyperlink ref="B231" location="_push_back_arrays" display="push_back_arrays"/>
+    <hyperlink ref="B235" location="_push_back_arrays" display="push_back_arrays"/>
     <hyperlink ref="B18" location="_find_imple" display="_find_imple"/>
+    <hyperlink ref="B207" location="_binary_less" display="binary_less"/>
+    <hyperlink ref="B208" location="_binary_less_dic" display="binary_less_dic"/>
+    <hyperlink ref="B209" location="_text_less" display="text_less"/>
+    <hyperlink ref="B210" location="_text_less_dic" display="text_less_dic"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
@@ -36078,12 +36402,12 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="219" spans="2:2" ht="409.6">
+    <row r="219" spans="2:2">
       <c r="B219" s="137" t="s">
         <v>1832</v>
       </c>
     </row>
-    <row r="220" spans="2:2" ht="409.6">
+    <row r="220" spans="2:2">
       <c r="B220" s="136" t="s">
         <v>1833</v>
       </c>
@@ -41734,7 +42058,7 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:B232"/>
+  <dimension ref="A1:B256"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -42700,30 +43024,107 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="225" spans="2:2">
+    <row r="225" spans="1:2">
       <c r="B225" s="12"/>
     </row>
-    <row r="226" spans="2:2" ht="14.25">
+    <row r="226" spans="1:2" ht="14.25">
       <c r="B226" s="62" t="s">
         <v>1876</v>
       </c>
     </row>
-    <row r="229" spans="2:2">
+    <row r="229" spans="1:2">
       <c r="B229" s="14" t="s">
         <v>1877</v>
       </c>
     </row>
-    <row r="230" spans="2:2" ht="14.25">
+    <row r="230" spans="1:2" ht="14.25">
       <c r="B230" s="14" t="s">
         <v>1878</v>
       </c>
     </row>
-    <row r="231" spans="2:2">
+    <row r="231" spans="1:2">
       <c r="B231" s="12"/>
     </row>
-    <row r="232" spans="2:2" ht="14.25">
+    <row r="232" spans="1:2" ht="14.25">
       <c r="B232" s="62" t="s">
         <v>1879</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="B235" s="14" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="14.25">
+      <c r="B236" s="14" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="B237" s="12"/>
+    </row>
+    <row r="238" spans="1:2" ht="14.25">
+      <c r="B238" s="62" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="17.25">
+      <c r="A240" s="21" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2">
+      <c r="B241" s="14" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2" ht="14.25">
+      <c r="B242" s="14" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2">
+      <c r="B243" s="12"/>
+    </row>
+    <row r="244" spans="2:2" ht="14.25">
+      <c r="B244" s="62" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="247" spans="2:2">
+      <c r="B247" s="14" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="248" spans="2:2" ht="14.25">
+      <c r="B248" s="14" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="249" spans="2:2">
+      <c r="B249" s="12"/>
+    </row>
+    <row r="250" spans="2:2" ht="14.25">
+      <c r="B250" s="62" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="253" spans="2:2">
+      <c r="B253" s="14" t="s">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="254" spans="2:2" ht="14.25">
+      <c r="B254" s="14" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="255" spans="2:2">
+      <c r="B255" s="12"/>
+    </row>
+    <row r="256" spans="2:2" ht="14.25">
+      <c r="B256" s="62" t="s">
+        <v>2052</v>
       </c>
     </row>
   </sheetData>
@@ -42739,6 +43140,7 @@
     <hyperlink ref="A175" location="_sorting" display="戻る"/>
     <hyperlink ref="A197" location="_sorting" display="戻る"/>
     <hyperlink ref="A221" location="_sorting" display="戻る"/>
+    <hyperlink ref="A240" location="_sorting" display="戻る"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>